<commit_message>
db med auto-refresh lagt til
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onedrive-global.kpmg.com/personal/joachim_svensson_kpmg_no/Documents/Desktop/projects/NorwegianHealthSector/Finnmarkssykehusene/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="641" documentId="11_F25DC773A252ABDACC10487AF99C75725BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03F1BFE8-3985-4C14-8D8F-15E840D77F01}"/>
+  <xr:revisionPtr revIDLastSave="642" documentId="11_F25DC773A252ABDACC10487AF99C75725BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{15F7EFA7-C102-4FDC-8411-A335422492F6}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bemanningsplan (2)" sheetId="5" r:id="rId1"/>
@@ -464,7 +464,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7492E8-5BAA-4205-8C79-80504931582E}">
   <dimension ref="A1:K46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
@@ -3805,8 +3805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E4017C6-41D0-4B5F-B3F7-48B94B162631}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3846,7 +3846,7 @@
         <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
login w/admin & customer functionality fixed
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onedrive-global.kpmg.com/personal/joachim_svensson_kpmg_no/Documents/Desktop/projects/NorwegianHealthSector/Finnmarkssykehusene/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="695" documentId="11_F25DC773A252ABDACC10487AF99C75725BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A733DB9-7848-4B0D-88CD-108611422B96}"/>
+  <xr:revisionPtr revIDLastSave="699" documentId="11_F25DC773A252ABDACC10487AF99C75725BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF537396-3170-47E5-BE1E-323CFE224352}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="døgnrytmetabell (2)" sheetId="6" r:id="rId1"/>
@@ -487,7 +487,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="A1:K49"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5987,7 +5987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
@@ -8638,8 +8638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E832C839-C4AE-402A-9328-3BE42A031A1A}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:K1"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -9530,7 +9530,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="C26">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D26">
         <v>3</v>
@@ -9600,25 +9600,25 @@
         <v>0.125</v>
       </c>
       <c r="C28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I28">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J28" t="s">
         <v>34</v>
@@ -9635,25 +9635,25 @@
         <v>0.16666666666666699</v>
       </c>
       <c r="C29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I29">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J29" t="s">
         <v>34</v>
@@ -9670,25 +9670,25 @@
         <v>0.20833333333333401</v>
       </c>
       <c r="C30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J30" t="s">
         <v>34</v>
@@ -9705,25 +9705,25 @@
         <v>0.25</v>
       </c>
       <c r="C31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="H31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I31">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J31" t="s">
         <v>34</v>
@@ -9740,25 +9740,25 @@
         <v>0.29166666666666702</v>
       </c>
       <c r="C32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I32">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J32" t="s">
         <v>34</v>
@@ -9775,25 +9775,25 @@
         <v>0.33333333333333398</v>
       </c>
       <c r="C33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="F33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I33">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J33" t="s">
         <v>34</v>
@@ -9810,25 +9810,25 @@
         <v>0.375</v>
       </c>
       <c r="C34">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D34">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E34">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F34">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G34">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H34">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I34">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J34" t="s">
         <v>34</v>
@@ -9845,25 +9845,25 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="C35">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D35">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="E35">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="F35">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G35">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H35">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="I35">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J35" t="s">
         <v>34</v>
@@ -9880,25 +9880,25 @@
         <v>0.45833333333333398</v>
       </c>
       <c r="C36">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D36">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E36">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F36">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G36">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H36">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I36">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J36" t="s">
         <v>34</v>
@@ -9915,25 +9915,25 @@
         <v>0.5</v>
       </c>
       <c r="C37">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D37">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E37">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F37">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G37">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H37">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I37">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J37" t="s">
         <v>34</v>
@@ -9965,10 +9965,10 @@
         <v>10</v>
       </c>
       <c r="H38">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I38">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J38" t="s">
         <v>34</v>
@@ -10067,7 +10067,7 @@
         <v>10</v>
       </c>
       <c r="G41">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H41">
         <v>10</v>
@@ -10102,7 +10102,7 @@
         <v>10</v>
       </c>
       <c r="G42">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H42">
         <v>10</v>
@@ -10125,25 +10125,25 @@
         <v>0.75</v>
       </c>
       <c r="C43">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D43">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E43">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F43">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G43">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H43">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I43">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J43" t="s">
         <v>34</v>
@@ -10160,25 +10160,25 @@
         <v>0.79166666666666696</v>
       </c>
       <c r="C44">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D44">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E44">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F44">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G44">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="H44">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I44">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J44" t="s">
         <v>34</v>
@@ -10207,7 +10207,7 @@
         <v>8</v>
       </c>
       <c r="G45">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H45">
         <v>8</v>
@@ -10230,25 +10230,25 @@
         <v>0.875</v>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G46">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I46">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J46" t="s">
         <v>34</v>
@@ -10265,25 +10265,25 @@
         <v>0.91666666666666696</v>
       </c>
       <c r="C47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I47">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J47" t="s">
         <v>34</v>
@@ -10300,25 +10300,25 @@
         <v>0.95833333333333404</v>
       </c>
       <c r="C48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I48">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J48" t="s">
         <v>34</v>
@@ -10353,7 +10353,7 @@
         <v>4</v>
       </c>
       <c r="I49">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J49" t="s">
         <v>34</v>

</xml_diff>

<commit_message>
azure deployment issues fixed
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onedrive-global.kpmg.com/personal/joachim_svensson_kpmg_no/Documents/Desktop/projects/NorwegianHealthSector/Finnmarkssykehusene/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="699" documentId="11_F25DC773A252ABDACC10487AF99C75725BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF537396-3170-47E5-BE1E-323CFE224352}"/>
+  <xr:revisionPtr revIDLastSave="701" documentId="11_F25DC773A252ABDACC10487AF99C75725BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6266AC42-9188-4639-855E-BA19F4FAC830}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8638,13 +8638,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E832C839-C4AE-402A-9328-3BE42A031A1A}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
deployed database oppdateringer - ny database i postgres
</commit_message>
<xml_diff>
--- a/test_data.xlsx
+++ b/test_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://onedrive-global.kpmg.com/personal/joachim_svensson_kpmg_no/Documents/Desktop/projects/NorwegianHealthSector/Finnmarkssykehusene/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="701" documentId="11_F25DC773A252ABDACC10487AF99C75725BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6266AC42-9188-4639-855E-BA19F4FAC830}"/>
+  <xr:revisionPtr revIDLastSave="708" documentId="11_F25DC773A252ABDACC10487AF99C75725BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D93EAD9-C137-4E35-9AE0-6713B7F2B070}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="døgnrytmetabell (2)" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="809" uniqueCount="41">
   <si>
     <t>Monday</t>
   </si>
@@ -156,6 +156,15 @@
   <si>
     <t>1-52</t>
   </si>
+  <si>
+    <t>Eksisterende</t>
+  </si>
+  <si>
+    <t>Forslag</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
 </sst>
 </file>
 
@@ -199,11 +208,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2232,17 +2244,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F7492E8-5BAA-4205-8C79-80504931582E}">
-  <dimension ref="A1:M91"/>
+  <dimension ref="A1:M101"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N96" sqref="N96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="5" max="5" width="10.6328125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8.7265625" style="1"/>
-    <col min="11" max="11" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.453125" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -5974,6 +5986,416 @@
         <v>34</v>
       </c>
       <c r="M91" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A92" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="B92" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C92" s="4">
+        <v>9</v>
+      </c>
+      <c r="D92" s="4">
+        <v>9</v>
+      </c>
+      <c r="E92" s="4">
+        <v>9</v>
+      </c>
+      <c r="F92" s="4">
+        <v>9</v>
+      </c>
+      <c r="G92" s="4">
+        <v>9</v>
+      </c>
+      <c r="H92" s="4">
+        <v>7</v>
+      </c>
+      <c r="I92" s="4">
+        <v>7</v>
+      </c>
+      <c r="J92" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K92" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L92" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M92" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A93" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="B93" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C93" s="4">
+        <v>8</v>
+      </c>
+      <c r="D93" s="4">
+        <v>8</v>
+      </c>
+      <c r="E93" s="4">
+        <v>8</v>
+      </c>
+      <c r="F93" s="4">
+        <v>8</v>
+      </c>
+      <c r="G93" s="4">
+        <v>8</v>
+      </c>
+      <c r="H93" s="4">
+        <v>6</v>
+      </c>
+      <c r="I93" s="4">
+        <v>6</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K93" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L93" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M93" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A94" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="B94" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C94" s="4">
+        <v>3</v>
+      </c>
+      <c r="D94" s="4">
+        <v>3</v>
+      </c>
+      <c r="E94" s="4">
+        <v>3</v>
+      </c>
+      <c r="F94" s="4">
+        <v>3</v>
+      </c>
+      <c r="G94" s="4">
+        <v>3</v>
+      </c>
+      <c r="H94" s="4">
+        <v>3</v>
+      </c>
+      <c r="I94" s="4">
+        <v>3</v>
+      </c>
+      <c r="J94" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K94" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="L94" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M94" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A95" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="B95" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C95" s="4">
+        <v>7</v>
+      </c>
+      <c r="D95" s="4">
+        <v>7</v>
+      </c>
+      <c r="E95" s="4">
+        <v>7</v>
+      </c>
+      <c r="F95" s="4">
+        <v>7</v>
+      </c>
+      <c r="G95" s="4">
+        <v>7</v>
+      </c>
+      <c r="H95" s="4">
+        <v>6</v>
+      </c>
+      <c r="I95" s="4">
+        <v>6</v>
+      </c>
+      <c r="J95" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K95" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L95" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M95" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A96" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="B96" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C96" s="4">
+        <v>6</v>
+      </c>
+      <c r="D96" s="4">
+        <v>6</v>
+      </c>
+      <c r="E96" s="4">
+        <v>6</v>
+      </c>
+      <c r="F96" s="4">
+        <v>6</v>
+      </c>
+      <c r="G96" s="4">
+        <v>6</v>
+      </c>
+      <c r="H96" s="4">
+        <v>5</v>
+      </c>
+      <c r="I96" s="4">
+        <v>5</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K96" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L96" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M96" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A97" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="B97" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C97" s="4">
+        <v>3</v>
+      </c>
+      <c r="D97" s="4">
+        <v>3</v>
+      </c>
+      <c r="E97" s="4">
+        <v>3</v>
+      </c>
+      <c r="F97" s="4">
+        <v>3</v>
+      </c>
+      <c r="G97" s="4">
+        <v>3</v>
+      </c>
+      <c r="H97" s="4">
+        <v>3</v>
+      </c>
+      <c r="I97" s="4">
+        <v>3</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K97" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="L97" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M97" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A98" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="B98" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="C98" s="4">
+        <v>6</v>
+      </c>
+      <c r="D98" s="4">
+        <v>6</v>
+      </c>
+      <c r="E98" s="4">
+        <v>6</v>
+      </c>
+      <c r="F98" s="4">
+        <v>6</v>
+      </c>
+      <c r="G98" s="4">
+        <v>6</v>
+      </c>
+      <c r="H98" s="4">
+        <v>5</v>
+      </c>
+      <c r="I98" s="4">
+        <v>5</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K98" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L98" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M98" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A99" s="2">
+        <v>0.625</v>
+      </c>
+      <c r="B99" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="C99" s="4">
+        <v>5</v>
+      </c>
+      <c r="D99" s="4">
+        <v>6</v>
+      </c>
+      <c r="E99" s="4">
+        <v>6</v>
+      </c>
+      <c r="F99" s="4">
+        <v>5</v>
+      </c>
+      <c r="G99" s="4">
+        <v>3</v>
+      </c>
+      <c r="H99" s="4">
+        <v>5</v>
+      </c>
+      <c r="I99" s="4">
+        <v>5</v>
+      </c>
+      <c r="J99" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K99" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L99" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M99" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A100" s="2">
+        <v>0.91666666666666663</v>
+      </c>
+      <c r="B100" s="2">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="C100" s="4">
+        <v>3</v>
+      </c>
+      <c r="D100" s="4">
+        <v>3</v>
+      </c>
+      <c r="E100" s="4">
+        <v>3</v>
+      </c>
+      <c r="F100" s="4">
+        <v>3</v>
+      </c>
+      <c r="G100" s="4">
+        <v>3</v>
+      </c>
+      <c r="H100" s="4">
+        <v>3</v>
+      </c>
+      <c r="I100" s="4">
+        <v>3</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K100" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L100" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M100" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A101" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="B101" s="2">
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="C101" s="4">
+        <v>2</v>
+      </c>
+      <c r="D101" s="4">
+        <v>2</v>
+      </c>
+      <c r="E101" s="4">
+        <v>2</v>
+      </c>
+      <c r="F101" s="4">
+        <v>2</v>
+      </c>
+      <c r="G101" s="4">
+        <v>2</v>
+      </c>
+      <c r="H101" s="4">
+        <v>1</v>
+      </c>
+      <c r="I101" s="4">
+        <v>1</v>
+      </c>
+      <c r="J101" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K101" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="L101" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M101" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -8638,8 +9060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E832C839-C4AE-402A-9328-3BE42A031A1A}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>